<commit_message>
feat: add orientation data handling and build orientation columns in batch laminate import
</commit_message>
<xml_diff>
--- a/Template Preenchido Upper Skin Grid_RevA.xlsx
+++ b/Template Preenchido Upper Skin Grid_RevA.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://embraer-my.sharepoint.com/personal/guilherme_rizzi_embraer_com_br/Documents/Documents/01-DIPAC_My Files/05-Skin Upper/06-Laminate/01-Laminate Optimization 21/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pribe\OneDrive\Documents\GitHub\GridLamEdit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE396D5F-B03F-4760-8959-DD2B558AD66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7E5B9C-B306-4076-960D-65A501A29AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Geral" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4461" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4454" uniqueCount="5">
   <si>
     <t>TAG</t>
   </si>
@@ -384,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,183 +430,6 @@
       <c r="J1">
         <v>7</v>
       </c>
-      <c r="K1">
-        <v>8</v>
-      </c>
-      <c r="L1">
-        <v>9</v>
-      </c>
-      <c r="M1">
-        <v>10</v>
-      </c>
-      <c r="N1">
-        <v>11</v>
-      </c>
-      <c r="O1">
-        <v>12</v>
-      </c>
-      <c r="P1">
-        <v>13</v>
-      </c>
-      <c r="Q1">
-        <v>14</v>
-      </c>
-      <c r="R1">
-        <v>15</v>
-      </c>
-      <c r="S1">
-        <v>16</v>
-      </c>
-      <c r="T1">
-        <v>17</v>
-      </c>
-      <c r="U1">
-        <v>18</v>
-      </c>
-      <c r="V1">
-        <v>19</v>
-      </c>
-      <c r="W1">
-        <v>20</v>
-      </c>
-      <c r="X1">
-        <v>21</v>
-      </c>
-      <c r="Y1">
-        <v>22</v>
-      </c>
-      <c r="Z1">
-        <v>23</v>
-      </c>
-      <c r="AA1">
-        <v>24</v>
-      </c>
-      <c r="AB1">
-        <v>25</v>
-      </c>
-      <c r="AC1">
-        <v>26</v>
-      </c>
-      <c r="AD1">
-        <v>27</v>
-      </c>
-      <c r="AE1">
-        <v>28</v>
-      </c>
-      <c r="AF1">
-        <v>29</v>
-      </c>
-      <c r="AG1">
-        <v>30</v>
-      </c>
-      <c r="AH1">
-        <v>31</v>
-      </c>
-      <c r="AI1">
-        <v>32</v>
-      </c>
-      <c r="AJ1">
-        <v>33</v>
-      </c>
-      <c r="AK1">
-        <v>34</v>
-      </c>
-      <c r="AL1">
-        <v>35</v>
-      </c>
-      <c r="AM1">
-        <v>36</v>
-      </c>
-      <c r="AN1">
-        <v>37</v>
-      </c>
-      <c r="AO1">
-        <v>38</v>
-      </c>
-      <c r="AP1">
-        <v>39</v>
-      </c>
-      <c r="AQ1">
-        <v>40</v>
-      </c>
-      <c r="AR1">
-        <v>41</v>
-      </c>
-      <c r="AS1">
-        <v>42</v>
-      </c>
-      <c r="AT1">
-        <v>43</v>
-      </c>
-      <c r="AU1">
-        <v>44</v>
-      </c>
-      <c r="AV1">
-        <v>45</v>
-      </c>
-      <c r="AW1">
-        <v>46</v>
-      </c>
-      <c r="AX1">
-        <v>47</v>
-      </c>
-      <c r="AY1">
-        <v>48</v>
-      </c>
-      <c r="AZ1" s="1">
-        <v>49</v>
-      </c>
-      <c r="BA1" s="1">
-        <v>50</v>
-      </c>
-      <c r="BB1" s="1">
-        <v>51</v>
-      </c>
-      <c r="BC1" s="1">
-        <v>52</v>
-      </c>
-      <c r="BD1" s="1">
-        <v>53</v>
-      </c>
-      <c r="BE1" s="1">
-        <v>54</v>
-      </c>
-      <c r="BF1" s="1">
-        <v>55</v>
-      </c>
-      <c r="BG1" s="1">
-        <v>56</v>
-      </c>
-      <c r="BH1" s="1">
-        <v>57</v>
-      </c>
-      <c r="BI1" s="1">
-        <v>58</v>
-      </c>
-      <c r="BJ1" s="1">
-        <v>59</v>
-      </c>
-      <c r="BK1" s="1">
-        <v>60</v>
-      </c>
-      <c r="BL1" s="1">
-        <v>61</v>
-      </c>
-      <c r="BM1" s="1">
-        <v>62</v>
-      </c>
-      <c r="BN1" s="1">
-        <v>63</v>
-      </c>
-      <c r="BO1" s="1">
-        <v>64</v>
-      </c>
-      <c r="BP1" s="1">
-        <v>65</v>
-      </c>
-      <c r="BQ1" s="1">
-        <v>66</v>
-      </c>
     </row>
     <row r="2" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -28412,9 +28235,6 @@
       <c r="B135" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D135" s="2">
         <v>45</v>
       </c>
@@ -28621,9 +28441,6 @@
       <c r="B136" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D136" s="2">
         <v>45</v>
       </c>
@@ -28830,9 +28647,6 @@
       <c r="B137" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D137" s="2">
         <v>45</v>
       </c>
@@ -29039,9 +28853,6 @@
       <c r="B138" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D138" s="2">
         <v>45</v>
       </c>
@@ -29248,9 +29059,6 @@
       <c r="B139" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D139" s="2">
         <v>45</v>
       </c>
@@ -29457,9 +29265,6 @@
       <c r="B140" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D140" s="2">
         <v>45</v>
       </c>
@@ -29664,9 +29469,6 @@
         <v>21322</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C141" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D141" s="2">

</xml_diff>